<commit_message>
take out state policy
</commit_message>
<xml_diff>
--- a/InputData/fuels/BCTR/BAU Carbon Tax Rate.xlsx
+++ b/InputData/fuels/BCTR/BAU Carbon Tax Rate.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11006"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olivia Ashmoore\Documents\EPS_Models by Region\RMI\RMI_all_states\PA\fuels\BCTR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/asonaike/Library/Containers/com.microsoft.Excel/Data/state-eps-data-repository/PA/fuels/BCTR/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7D67351C-9639-4C40-8616-413D899F0A30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B3AB48A6-C35A-6845-8868-8A138D46DF96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1415" yWindow="1415" windowWidth="14400" windowHeight="7290" activeTab="1" xr2:uid="{061459C3-F8E3-40F7-8A92-425A32688CAD}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="5" xr2:uid="{061459C3-F8E3-40F7-8A92-425A32688CAD}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="RGGI" sheetId="23" r:id="rId2"/>
-    <sheet name="CA" sheetId="19" r:id="rId3"/>
-    <sheet name="state calcs" sheetId="20" r:id="rId4"/>
-    <sheet name="BCTR" sheetId="2" r:id="rId5"/>
+    <sheet name="WA" sheetId="24" r:id="rId3"/>
+    <sheet name="CA" sheetId="19" r:id="rId4"/>
+    <sheet name="state calcs" sheetId="20" r:id="rId5"/>
+    <sheet name="BCTR" sheetId="2" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="HHV_Adjust">#REF!</definedName>
@@ -65,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="272">
   <si>
     <t>BCTR BAU Carbon Tax Rate</t>
   </si>
@@ -857,6 +858,30 @@
   </si>
   <si>
     <t>2023............................................................................. .</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>$/MMT CO2e</t>
+  </si>
+  <si>
+    <t>Washington - values from RMI reflecting Washington state predicted carbon allowance prices</t>
+  </si>
+  <si>
+    <t>Sectors:</t>
+  </si>
+  <si>
+    <t>fuel suppliers, natural gas and electric utilities, waste-to-energy facilities (starting in 2027), and railroads (starting in 2031).</t>
+  </si>
+  <si>
+    <t>https://ecology.wa.gov/air-climate/climate-commitment-act/cap-and-invest</t>
+  </si>
+  <si>
+    <t>https://apps.ecology.wa.gov/publications/documents/2302010.pdf</t>
+  </si>
+  <si>
+    <t>&lt;-- nearly 100% free allowances until 2034</t>
   </si>
 </sst>
 </file>
@@ -873,7 +898,7 @@
     <numFmt numFmtId="166" formatCode="_(* #,##0.000_);_(* \(#,##0.000\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="167" formatCode="0.000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -916,8 +941,42 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF1D1C1D"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF1D1C1D"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -972,6 +1031,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="4">
     <border>
@@ -1019,12 +1084,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1068,10 +1134,17 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="4">
@@ -4999,16 +5072,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>601662</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>14287</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>201612</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>138112</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>296862</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>134937</xdr:rowOff>
+      <xdr:colOff>506412</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>68262</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5335,13 +5408,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49357908-BC85-41CC-9D98-173369A13AF6}">
   <dimension ref="A1:M51"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5349,7 +5422,7 @@
         <v>138</v>
       </c>
       <c r="C1" s="18">
-        <v>45501</v>
+        <v>45576</v>
       </c>
       <c r="D1" s="19"/>
       <c r="E1" s="19"/>
@@ -5367,7 +5440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B2" s="19" t="str">
         <f>LOOKUP(B1,K1:L51,L1:L51)</f>
         <v>PA</v>
@@ -5389,7 +5462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -5406,7 +5479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>12</v>
       </c>
@@ -5420,7 +5493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="K5" s="17" t="s">
         <v>73</v>
       </c>
@@ -5431,7 +5504,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>15</v>
       </c>
@@ -5445,7 +5518,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>19</v>
       </c>
@@ -5459,7 +5532,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>13</v>
       </c>
@@ -5473,7 +5546,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>14</v>
       </c>
@@ -5487,7 +5560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
       <c r="K10" s="17" t="s">
         <v>83</v>
@@ -5499,7 +5572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
       <c r="B11" t="s">
         <v>26</v>
@@ -5514,7 +5587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="B12" t="s">
         <v>27</v>
@@ -5529,7 +5602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>25</v>
       </c>
@@ -5543,7 +5616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="K14" s="17" t="s">
         <v>90</v>
@@ -5555,7 +5628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>246</v>
       </c>
@@ -5569,7 +5642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>247</v>
       </c>
@@ -5583,7 +5656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B17">
         <v>2023</v>
       </c>
@@ -5597,7 +5670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>248</v>
       </c>
@@ -5611,7 +5684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="K19" s="17" t="s">
         <v>100</v>
       </c>
@@ -5622,7 +5695,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>266</v>
+      </c>
       <c r="K20" s="17" t="s">
         <v>102</v>
       </c>
@@ -5633,7 +5709,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>270</v>
+      </c>
       <c r="K21" s="17" t="s">
         <v>104</v>
       </c>
@@ -5644,7 +5723,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="K22" s="17" t="s">
         <v>106</v>
       </c>
@@ -5655,7 +5734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="K23" s="17" t="s">
         <v>108</v>
       </c>
@@ -5666,7 +5745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>2</v>
       </c>
@@ -5680,7 +5759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -5694,7 +5773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>20</v>
       </c>
@@ -5708,7 +5787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>21</v>
       </c>
@@ -5722,7 +5801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
         <v>22</v>
       </c>
@@ -5736,7 +5815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="K29" s="17" t="s">
         <v>120</v>
       </c>
@@ -5747,7 +5826,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>24</v>
       </c>
@@ -5761,7 +5840,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="K31" s="17" t="s">
         <v>124</v>
       </c>
@@ -5772,7 +5851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>61</v>
       </c>
@@ -5786,7 +5865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>16</v>
       </c>
@@ -5803,7 +5882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>17</v>
       </c>
@@ -5820,7 +5899,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>18</v>
       </c>
@@ -5837,7 +5916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>59</v>
       </c>
@@ -5854,7 +5933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>60</v>
       </c>
@@ -5871,7 +5950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>263</v>
       </c>
@@ -5888,11 +5967,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="K39" s="17"/>
       <c r="L39" s="17"/>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>255</v>
       </c>
@@ -5906,7 +5985,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="K41" s="17" t="s">
         <v>142</v>
       </c>
@@ -5917,7 +5996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="K42" s="17" t="s">
         <v>144</v>
       </c>
@@ -5928,7 +6007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="K43" s="17" t="s">
         <v>146</v>
       </c>
@@ -5939,7 +6018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="K44" s="17" t="s">
         <v>148</v>
       </c>
@@ -5950,7 +6029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="K45" s="17" t="s">
         <v>150</v>
       </c>
@@ -5961,7 +6040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="K46" s="17" t="s">
         <v>152</v>
       </c>
@@ -5972,7 +6051,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="K47" s="17" t="s">
         <v>154</v>
       </c>
@@ -5983,7 +6062,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="K48" s="17" t="s">
         <v>156</v>
       </c>
@@ -5994,7 +6073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="11:13" x14ac:dyDescent="0.75">
+    <row r="49" spans="11:13" x14ac:dyDescent="0.2">
       <c r="K49" s="17" t="s">
         <v>158</v>
       </c>
@@ -6005,7 +6084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="11:13" x14ac:dyDescent="0.75">
+    <row r="50" spans="11:13" x14ac:dyDescent="0.2">
       <c r="K50" s="17" t="s">
         <v>160</v>
       </c>
@@ -6016,7 +6095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="11:13" x14ac:dyDescent="0.75">
+    <row r="51" spans="11:13" x14ac:dyDescent="0.2">
       <c r="K51" s="17" t="s">
         <v>162</v>
       </c>
@@ -6051,20 +6130,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74D73BFE-C2AD-46BA-8005-FEF65B146DAA}">
   <dimension ref="A1:M78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="10.81640625" customWidth="1"/>
-    <col min="3" max="3" width="10.26953125" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.1796875" customWidth="1"/>
-    <col min="13" max="13" width="14.7265625" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.1640625" customWidth="1"/>
+    <col min="13" max="13" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>254</v>
       </c>
@@ -6072,7 +6151,7 @@
         <v>0.90718500000000002</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="59" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>164</v>
       </c>
@@ -6101,7 +6180,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2024</v>
       </c>
@@ -6138,7 +6217,7 @@
         <v>9.2213188678974873</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2024</v>
       </c>
@@ -6175,7 +6254,7 @@
         <v>9.5795587797898545</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2023</v>
       </c>
@@ -6212,7 +6291,7 @@
         <v>7.2773036678823289</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2023</v>
       </c>
@@ -6249,7 +6328,7 @@
         <v>5.15658616613156</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2023</v>
       </c>
@@ -6286,7 +6365,7 @@
         <v>4.4197575792106214</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2023</v>
       </c>
@@ -6323,7 +6402,7 @@
         <v>3.6620838455692195</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2022</v>
       </c>
@@ -6349,7 +6428,7 @@
         <v>288809306.97000003</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2022</v>
       </c>
@@ -6382,7 +6461,7 @@
         <v>1.2970370347179943</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2022</v>
       </c>
@@ -6415,7 +6494,7 @@
         <v>-2614.1105604966269</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2022</v>
       </c>
@@ -6441,7 +6520,7 @@
         <v>293777131.5</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2021</v>
       </c>
@@ -6471,7 +6550,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2021</v>
       </c>
@@ -6504,7 +6583,7 @@
         <v>3.6620838455692195</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2021</v>
       </c>
@@ -6537,7 +6616,7 @@
         <v>4.4197575792106214</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2021</v>
       </c>
@@ -6570,7 +6649,7 @@
         <v>5.15658616613156</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2020</v>
       </c>
@@ -6603,7 +6682,7 @@
         <v>7.2773036678823289</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>2020</v>
       </c>
@@ -6636,7 +6715,7 @@
         <v>9.5795587797898545</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2020</v>
       </c>
@@ -6669,7 +6748,7 @@
         <v>9.2213188678974873</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2020</v>
       </c>
@@ -6702,7 +6781,7 @@
         <v>11.092397772593358</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>2019</v>
       </c>
@@ -6735,7 +6814,7 @@
         <v>12.389434807311318</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>2019</v>
       </c>
@@ -6768,7 +6847,7 @@
         <v>13.686471842029277</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>2019</v>
       </c>
@@ -6801,7 +6880,7 @@
         <v>14.983508876747237</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>2019</v>
       </c>
@@ -6834,7 +6913,7 @@
         <v>16.280545911465197</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>2018</v>
       </c>
@@ -6867,7 +6946,7 @@
         <v>17.577582946183611</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>2018</v>
       </c>
@@ -6900,7 +6979,7 @@
         <v>18.874619980901571</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>2018</v>
       </c>
@@ -6933,7 +7012,7 @@
         <v>20.17165701561953</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>2018</v>
       </c>
@@ -6966,7 +7045,7 @@
         <v>21.46869405033749</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>194</v>
       </c>
@@ -6996,7 +7075,7 @@
         <v>22.76573108505545</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>195</v>
       </c>
@@ -7026,7 +7105,7 @@
         <v>24.062768119773409</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>196</v>
       </c>
@@ -7056,7 +7135,7 @@
         <v>25.359805154491369</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>197</v>
       </c>
@@ -7086,7 +7165,7 @@
         <v>26.656842189209328</v>
       </c>
     </row>
-    <row r="33" spans="2:12" x14ac:dyDescent="0.75">
+    <row r="33" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>198</v>
       </c>
@@ -7116,7 +7195,7 @@
         <v>27.953879223927288</v>
       </c>
     </row>
-    <row r="34" spans="2:12" x14ac:dyDescent="0.75">
+    <row r="34" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
         <v>199</v>
       </c>
@@ -7146,7 +7225,7 @@
         <v>29.250916258645248</v>
       </c>
     </row>
-    <row r="35" spans="2:12" x14ac:dyDescent="0.75">
+    <row r="35" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
         <v>200</v>
       </c>
@@ -7176,7 +7255,7 @@
         <v>30.547953293363207</v>
       </c>
     </row>
-    <row r="36" spans="2:12" x14ac:dyDescent="0.75">
+    <row r="36" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
         <v>201</v>
       </c>
@@ -7206,7 +7285,7 @@
         <v>31.844990328081167</v>
       </c>
     </row>
-    <row r="37" spans="2:12" x14ac:dyDescent="0.75">
+    <row r="37" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
         <v>202</v>
       </c>
@@ -7236,7 +7315,7 @@
         <v>33.142027362799126</v>
       </c>
     </row>
-    <row r="38" spans="2:12" x14ac:dyDescent="0.75">
+    <row r="38" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
         <v>203</v>
       </c>
@@ -7266,7 +7345,7 @@
         <v>34.439064397517541</v>
       </c>
     </row>
-    <row r="39" spans="2:12" x14ac:dyDescent="0.75">
+    <row r="39" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
         <v>204</v>
       </c>
@@ -7296,7 +7375,7 @@
         <v>35.7361014322355</v>
       </c>
     </row>
-    <row r="40" spans="2:12" x14ac:dyDescent="0.75">
+    <row r="40" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
         <v>205</v>
       </c>
@@ -7326,7 +7405,7 @@
         <v>37.03313846695346</v>
       </c>
     </row>
-    <row r="41" spans="2:12" x14ac:dyDescent="0.75">
+    <row r="41" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
         <v>206</v>
       </c>
@@ -7356,7 +7435,7 @@
         <v>38.33017550167142</v>
       </c>
     </row>
-    <row r="42" spans="2:12" x14ac:dyDescent="0.75">
+    <row r="42" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
         <v>207</v>
       </c>
@@ -7386,7 +7465,7 @@
         <v>39.627212536389379</v>
       </c>
     </row>
-    <row r="43" spans="2:12" x14ac:dyDescent="0.75">
+    <row r="43" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
         <v>208</v>
       </c>
@@ -7416,7 +7495,7 @@
         <v>40.924249571107339</v>
       </c>
     </row>
-    <row r="44" spans="2:12" x14ac:dyDescent="0.75">
+    <row r="44" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
         <v>209</v>
       </c>
@@ -7446,7 +7525,7 @@
         <v>42.221286605825298</v>
       </c>
     </row>
-    <row r="45" spans="2:12" x14ac:dyDescent="0.75">
+    <row r="45" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
         <v>210</v>
       </c>
@@ -7476,7 +7555,7 @@
         <v>43.518323640543258</v>
       </c>
     </row>
-    <row r="46" spans="2:12" x14ac:dyDescent="0.75">
+    <row r="46" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
         <v>212</v>
       </c>
@@ -7506,7 +7585,7 @@
         <v>44.815360675261218</v>
       </c>
     </row>
-    <row r="47" spans="2:12" x14ac:dyDescent="0.75">
+    <row r="47" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
         <v>213</v>
       </c>
@@ -7529,7 +7608,7 @@
         <v>124490463.95999999</v>
       </c>
     </row>
-    <row r="48" spans="2:12" x14ac:dyDescent="0.75">
+    <row r="48" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
         <v>214</v>
       </c>
@@ -7552,7 +7631,7 @@
         <v>105939134</v>
       </c>
     </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.75">
+    <row r="49" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
         <v>215</v>
       </c>
@@ -7575,7 +7654,7 @@
         <v>38163820</v>
       </c>
     </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.75">
+    <row r="50" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
         <v>216</v>
       </c>
@@ -7598,7 +7677,7 @@
         <v>47456770</v>
       </c>
     </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.75">
+    <row r="51" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
         <v>217</v>
       </c>
@@ -7621,7 +7700,7 @@
         <v>40416130</v>
       </c>
     </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.75">
+    <row r="52" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
         <v>218</v>
       </c>
@@ -7644,7 +7723,7 @@
         <v>41608870</v>
       </c>
     </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.75">
+    <row r="53" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
         <v>219</v>
       </c>
@@ -7667,7 +7746,7 @@
         <v>51583770</v>
       </c>
     </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.75">
+    <row r="54" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
         <v>220</v>
       </c>
@@ -7690,7 +7769,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.75">
+    <row r="55" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
         <v>221</v>
       </c>
@@ -7713,7 +7792,7 @@
         <v>14150430</v>
       </c>
     </row>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.75">
+    <row r="56" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B56" t="s">
         <v>222</v>
       </c>
@@ -7736,7 +7815,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="57" spans="2:8" x14ac:dyDescent="0.75">
+    <row r="57" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B57" t="s">
         <v>223</v>
       </c>
@@ -7759,7 +7838,7 @@
         <v>25477200</v>
       </c>
     </row>
-    <row r="58" spans="2:8" x14ac:dyDescent="0.75">
+    <row r="58" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B58" t="s">
         <v>224</v>
       </c>
@@ -7782,7 +7861,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="59" spans="2:8" x14ac:dyDescent="0.75">
+    <row r="59" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B59" t="s">
         <v>225</v>
       </c>
@@ -7805,7 +7884,7 @@
         <v>83425588.469999999</v>
       </c>
     </row>
-    <row r="60" spans="2:8" x14ac:dyDescent="0.75">
+    <row r="60" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B60" t="s">
         <v>226</v>
       </c>
@@ -7828,7 +7907,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="61" spans="2:8" x14ac:dyDescent="0.75">
+    <row r="61" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B61" t="s">
         <v>227</v>
       </c>
@@ -7851,7 +7930,7 @@
         <v>48224220</v>
       </c>
     </row>
-    <row r="62" spans="2:8" x14ac:dyDescent="0.75">
+    <row r="62" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B62" t="s">
         <v>228</v>
       </c>
@@ -7874,7 +7953,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="63" spans="2:8" x14ac:dyDescent="0.75">
+    <row r="63" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B63" t="s">
         <v>229</v>
       </c>
@@ -7897,7 +7976,7 @@
         <v>66437340</v>
       </c>
     </row>
-    <row r="64" spans="2:8" x14ac:dyDescent="0.75">
+    <row r="64" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B64" t="s">
         <v>230</v>
       </c>
@@ -7920,7 +7999,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="65" spans="2:8" x14ac:dyDescent="0.75">
+    <row r="65" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B65" t="s">
         <v>231</v>
       </c>
@@ -7943,7 +8022,7 @@
         <v>80465566.780000001</v>
       </c>
     </row>
-    <row r="66" spans="2:8" x14ac:dyDescent="0.75">
+    <row r="66" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B66" t="s">
         <v>232</v>
       </c>
@@ -7966,7 +8045,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="67" spans="2:8" x14ac:dyDescent="0.75">
+    <row r="67" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B67" t="s">
         <v>233</v>
       </c>
@@ -7989,7 +8068,7 @@
         <v>87956944.560000002</v>
       </c>
     </row>
-    <row r="68" spans="2:8" x14ac:dyDescent="0.75">
+    <row r="68" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B68" t="s">
         <v>234</v>
       </c>
@@ -8012,7 +8091,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="69" spans="2:8" x14ac:dyDescent="0.75">
+    <row r="69" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B69" t="s">
         <v>235</v>
       </c>
@@ -8035,7 +8114,7 @@
         <v>61587120.899999999</v>
       </c>
     </row>
-    <row r="70" spans="2:8" x14ac:dyDescent="0.75">
+    <row r="70" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B70" t="s">
         <v>236</v>
       </c>
@@ -8058,7 +8137,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="71" spans="2:8" x14ac:dyDescent="0.75">
+    <row r="71" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B71" t="s">
         <v>237</v>
       </c>
@@ -8081,7 +8160,7 @@
         <v>66278239.350000001</v>
       </c>
     </row>
-    <row r="72" spans="2:8" x14ac:dyDescent="0.75">
+    <row r="72" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B72" t="s">
         <v>238</v>
       </c>
@@ -8104,7 +8183,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="73" spans="2:8" x14ac:dyDescent="0.75">
+    <row r="73" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B73" t="s">
         <v>239</v>
       </c>
@@ -8127,7 +8206,7 @@
         <v>104242445</v>
       </c>
     </row>
-    <row r="74" spans="2:8" x14ac:dyDescent="0.75">
+    <row r="74" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B74" t="s">
         <v>240</v>
       </c>
@@ -8150,7 +8229,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="75" spans="2:8" x14ac:dyDescent="0.75">
+    <row r="75" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B75" t="s">
         <v>241</v>
       </c>
@@ -8173,7 +8252,7 @@
         <v>117248629.8</v>
       </c>
     </row>
-    <row r="76" spans="2:8" x14ac:dyDescent="0.75">
+    <row r="76" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B76" t="s">
         <v>242</v>
       </c>
@@ -8196,7 +8275,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="77" spans="2:8" x14ac:dyDescent="0.75">
+    <row r="77" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B77" t="s">
         <v>243</v>
       </c>
@@ -8219,7 +8298,7 @@
         <v>106489935.23999999</v>
       </c>
     </row>
-    <row r="78" spans="2:8" x14ac:dyDescent="0.75">
+    <row r="78" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B78" t="s">
         <v>244</v>
       </c>
@@ -8248,35 +8327,266 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E50BEE71-F449-4B9C-A073-79C961EF0E05}">
+  <dimension ref="A1:AC13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" s="42" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="41" t="s">
+        <v>264</v>
+      </c>
+      <c r="B1" s="41">
+        <v>2023</v>
+      </c>
+      <c r="C1" s="41">
+        <v>2024</v>
+      </c>
+      <c r="D1" s="41">
+        <v>2025</v>
+      </c>
+      <c r="E1" s="41">
+        <v>2026</v>
+      </c>
+      <c r="F1" s="41">
+        <v>2027</v>
+      </c>
+      <c r="G1" s="41">
+        <v>2028</v>
+      </c>
+      <c r="H1" s="41">
+        <v>2029</v>
+      </c>
+      <c r="I1" s="41">
+        <v>2030</v>
+      </c>
+      <c r="J1" s="41">
+        <v>2031</v>
+      </c>
+      <c r="K1" s="41">
+        <v>2032</v>
+      </c>
+      <c r="L1" s="41">
+        <v>2033</v>
+      </c>
+      <c r="M1" s="41">
+        <v>2034</v>
+      </c>
+      <c r="N1" s="41">
+        <v>2035</v>
+      </c>
+      <c r="O1" s="41">
+        <v>2036</v>
+      </c>
+      <c r="P1" s="41">
+        <v>2037</v>
+      </c>
+      <c r="Q1" s="41">
+        <v>2038</v>
+      </c>
+      <c r="R1" s="41">
+        <v>2039</v>
+      </c>
+      <c r="S1" s="41">
+        <v>2040</v>
+      </c>
+      <c r="T1" s="41">
+        <v>2041</v>
+      </c>
+      <c r="U1" s="41">
+        <v>2042</v>
+      </c>
+      <c r="V1" s="41">
+        <v>2043</v>
+      </c>
+      <c r="W1" s="41">
+        <v>2044</v>
+      </c>
+      <c r="X1" s="41">
+        <v>2045</v>
+      </c>
+      <c r="Y1" s="41">
+        <v>2046</v>
+      </c>
+      <c r="Z1" s="41">
+        <v>2047</v>
+      </c>
+      <c r="AA1" s="41">
+        <v>2048</v>
+      </c>
+      <c r="AB1" s="41">
+        <v>2049</v>
+      </c>
+      <c r="AC1" s="41">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" s="42" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="42" t="s">
+        <v>265</v>
+      </c>
+      <c r="B2" s="42">
+        <v>58</v>
+      </c>
+      <c r="C2" s="42">
+        <v>64</v>
+      </c>
+      <c r="D2" s="42">
+        <v>70</v>
+      </c>
+      <c r="E2" s="42">
+        <v>76</v>
+      </c>
+      <c r="F2" s="42">
+        <v>82</v>
+      </c>
+      <c r="G2" s="42">
+        <v>88</v>
+      </c>
+      <c r="H2" s="42">
+        <v>94</v>
+      </c>
+      <c r="I2" s="42">
+        <v>100</v>
+      </c>
+      <c r="J2" s="42">
+        <v>100</v>
+      </c>
+      <c r="K2" s="42">
+        <v>100</v>
+      </c>
+      <c r="L2" s="42">
+        <v>100</v>
+      </c>
+      <c r="M2" s="42">
+        <v>100</v>
+      </c>
+      <c r="N2" s="42">
+        <v>58</v>
+      </c>
+      <c r="O2" s="42">
+        <v>54.4</v>
+      </c>
+      <c r="P2" s="42">
+        <v>50.8</v>
+      </c>
+      <c r="Q2" s="42">
+        <v>47.2</v>
+      </c>
+      <c r="R2" s="42">
+        <v>43.6</v>
+      </c>
+      <c r="S2" s="42">
+        <v>40</v>
+      </c>
+      <c r="T2" s="42">
+        <v>44</v>
+      </c>
+      <c r="U2" s="42">
+        <v>48</v>
+      </c>
+      <c r="V2" s="42">
+        <v>52</v>
+      </c>
+      <c r="W2" s="42">
+        <v>56</v>
+      </c>
+      <c r="X2" s="42">
+        <v>60</v>
+      </c>
+      <c r="Y2" s="42">
+        <v>64</v>
+      </c>
+      <c r="Z2" s="42">
+        <v>68</v>
+      </c>
+      <c r="AA2" s="42">
+        <v>72</v>
+      </c>
+      <c r="AB2" s="42">
+        <v>76</v>
+      </c>
+      <c r="AC2" s="42">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A4" s="37"/>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="39" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A9" s="40" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A11" s="37"/>
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A12" s="37"/>
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A13" s="37"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A9" r:id="rId1" xr:uid="{6D7ECB27-F57E-4E70-AC08-F45980D501B7}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81A98054-2B91-4DE7-AD82-A1CFC0A86BB0}">
   <dimension ref="A1:H74"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="30.1796875" customWidth="1"/>
+    <col min="2" max="2" width="30.1640625" customWidth="1"/>
     <col min="3" max="8" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="59" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:8" ht="64" x14ac:dyDescent="0.2">
       <c r="B5" s="12" t="s">
         <v>29</v>
       </c>
@@ -8299,7 +8609,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="13">
         <v>2024</v>
       </c>
@@ -8325,7 +8635,7 @@
         <v>38.35</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="13">
         <v>2024</v>
       </c>
@@ -8351,7 +8661,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="13">
         <v>2023</v>
       </c>
@@ -8377,7 +8687,7 @@
         <v>37.4</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="13">
         <v>2023</v>
       </c>
@@ -8403,7 +8713,7 @@
         <v>34.159999999999997</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="13">
         <v>2023</v>
       </c>
@@ -8429,7 +8739,7 @@
         <v>30.05</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="13">
         <v>2023</v>
       </c>
@@ -8455,7 +8765,7 @@
         <v>27.01</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="13">
         <v>2022</v>
       </c>
@@ -8481,7 +8791,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="13">
         <v>2022</v>
       </c>
@@ -8507,7 +8817,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="13">
         <v>2022</v>
       </c>
@@ -8533,7 +8843,7 @@
         <v>28.13</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="13">
         <v>2022</v>
       </c>
@@ -8559,7 +8869,7 @@
         <v>19.7</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="13">
         <v>2021</v>
       </c>
@@ -8585,7 +8895,7 @@
         <v>34.01</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="13">
         <v>2021</v>
       </c>
@@ -8611,7 +8921,7 @@
         <v>23.69</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="13">
         <v>2021</v>
       </c>
@@ -8637,7 +8947,7 @@
         <v>19.04</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="13">
         <v>2021</v>
       </c>
@@ -8663,7 +8973,7 @@
         <v>18.010000000000002</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="13">
         <v>2020</v>
       </c>
@@ -8689,7 +8999,7 @@
         <v>17.350000000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="13">
         <v>2020</v>
       </c>
@@ -8715,7 +9025,7 @@
         <v>16.73</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="13">
         <v>2020</v>
       </c>
@@ -8741,7 +9051,7 @@
         <v>16.68</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="13">
         <v>2020</v>
       </c>
@@ -8767,7 +9077,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="13">
         <v>2019</v>
       </c>
@@ -8793,7 +9103,7 @@
         <v>16.8</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="13">
         <v>2019</v>
       </c>
@@ -8819,7 +9129,7 @@
         <v>16.850000000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="13">
         <v>2019</v>
       </c>
@@ -8845,7 +9155,7 @@
         <v>17.399999999999999</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="13">
         <v>2019</v>
       </c>
@@ -8871,7 +9181,7 @@
         <v>15.62</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="13">
         <v>2018</v>
       </c>
@@ -8897,7 +9207,7 @@
         <v>15.33</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="13">
         <v>2018</v>
       </c>
@@ -8923,7 +9233,7 @@
         <v>14.9</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="32" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="C32" s="1" t="s">
         <v>57</v>
       </c>
@@ -8937,7 +9247,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="33" spans="4:7" x14ac:dyDescent="0.75">
+    <row r="33" spans="4:7" x14ac:dyDescent="0.2">
       <c r="D33" s="1">
         <v>2018</v>
       </c>
@@ -8954,7 +9264,7 @@
         <v>2.2912872296992677</v>
       </c>
     </row>
-    <row r="34" spans="4:7" x14ac:dyDescent="0.75">
+    <row r="34" spans="4:7" x14ac:dyDescent="0.2">
       <c r="D34" s="1">
         <v>2019</v>
       </c>
@@ -8971,7 +9281,7 @@
         <v>-4611.2133228755793</v>
       </c>
     </row>
-    <row r="35" spans="4:7" x14ac:dyDescent="0.75">
+    <row r="35" spans="4:7" x14ac:dyDescent="0.2">
       <c r="D35" s="1">
         <v>2020</v>
       </c>
@@ -8984,7 +9294,7 @@
         <v>15.116365842255545</v>
       </c>
     </row>
-    <row r="36" spans="4:7" x14ac:dyDescent="0.75">
+    <row r="36" spans="4:7" x14ac:dyDescent="0.2">
       <c r="D36" s="1">
         <v>2021</v>
       </c>
@@ -8997,7 +9307,7 @@
         <v>18.674583016570097</v>
       </c>
     </row>
-    <row r="37" spans="4:7" x14ac:dyDescent="0.75">
+    <row r="37" spans="4:7" x14ac:dyDescent="0.2">
       <c r="D37" s="1">
         <v>2022</v>
       </c>
@@ -9010,7 +9320,7 @@
         <v>22.319623105704672</v>
       </c>
     </row>
-    <row r="38" spans="4:7" x14ac:dyDescent="0.75">
+    <row r="38" spans="4:7" x14ac:dyDescent="0.2">
       <c r="D38" s="1">
         <v>2023</v>
       </c>
@@ -9023,7 +9333,7 @@
         <v>24.886334303680318</v>
       </c>
     </row>
-    <row r="39" spans="4:7" x14ac:dyDescent="0.75">
+    <row r="39" spans="4:7" x14ac:dyDescent="0.2">
       <c r="D39" s="1">
         <v>2024</v>
       </c>
@@ -9036,13 +9346,13 @@
         <v>29.680499832623351</v>
       </c>
     </row>
-    <row r="41" spans="4:7" x14ac:dyDescent="0.75">
+    <row r="41" spans="4:7" x14ac:dyDescent="0.2">
       <c r="D41" s="28"/>
       <c r="E41" s="30" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="42" spans="4:7" x14ac:dyDescent="0.75">
+    <row r="42" spans="4:7" x14ac:dyDescent="0.2">
       <c r="D42" s="30">
         <v>2018</v>
       </c>
@@ -9051,7 +9361,7 @@
         <v>13.879489301373518</v>
       </c>
     </row>
-    <row r="43" spans="4:7" x14ac:dyDescent="0.75">
+    <row r="43" spans="4:7" x14ac:dyDescent="0.2">
       <c r="D43" s="30">
         <v>2019</v>
       </c>
@@ -9060,7 +9370,7 @@
         <v>15.11875282116273</v>
       </c>
     </row>
-    <row r="44" spans="4:7" x14ac:dyDescent="0.75">
+    <row r="44" spans="4:7" x14ac:dyDescent="0.2">
       <c r="D44" s="30">
         <v>2020</v>
       </c>
@@ -9069,7 +9379,7 @@
         <v>15.116365842255545</v>
       </c>
     </row>
-    <row r="45" spans="4:7" x14ac:dyDescent="0.75">
+    <row r="45" spans="4:7" x14ac:dyDescent="0.2">
       <c r="D45" s="30">
         <v>2021</v>
       </c>
@@ -9078,7 +9388,7 @@
         <v>18.674583016570097</v>
       </c>
     </row>
-    <row r="46" spans="4:7" x14ac:dyDescent="0.75">
+    <row r="46" spans="4:7" x14ac:dyDescent="0.2">
       <c r="D46" s="30">
         <v>2022</v>
       </c>
@@ -9087,7 +9397,7 @@
         <v>22.319623105704672</v>
       </c>
     </row>
-    <row r="47" spans="4:7" x14ac:dyDescent="0.75">
+    <row r="47" spans="4:7" x14ac:dyDescent="0.2">
       <c r="D47" s="30">
         <v>2023</v>
       </c>
@@ -9096,7 +9406,7 @@
         <v>24.886334303680318</v>
       </c>
     </row>
-    <row r="48" spans="4:7" x14ac:dyDescent="0.75">
+    <row r="48" spans="4:7" x14ac:dyDescent="0.2">
       <c r="D48" s="30">
         <v>2024</v>
       </c>
@@ -9105,7 +9415,7 @@
         <v>29.680499832623351</v>
       </c>
     </row>
-    <row r="49" spans="4:5" x14ac:dyDescent="0.75">
+    <row r="49" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D49" s="30">
         <v>2025</v>
       </c>
@@ -9114,7 +9424,7 @@
         <v>28.643317265437872</v>
       </c>
     </row>
-    <row r="50" spans="4:5" x14ac:dyDescent="0.75">
+    <row r="50" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D50" s="30">
         <v>2026</v>
       </c>
@@ -9123,7 +9433,7 @@
         <v>30.934604495137137</v>
       </c>
     </row>
-    <row r="51" spans="4:5" x14ac:dyDescent="0.75">
+    <row r="51" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D51" s="30">
         <v>2027</v>
       </c>
@@ -9132,7 +9442,7 @@
         <v>33.225891724836401</v>
       </c>
     </row>
-    <row r="52" spans="4:5" x14ac:dyDescent="0.75">
+    <row r="52" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D52" s="30">
         <v>2028</v>
       </c>
@@ -9141,7 +9451,7 @@
         <v>35.517178954535666</v>
       </c>
     </row>
-    <row r="53" spans="4:5" x14ac:dyDescent="0.75">
+    <row r="53" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D53" s="30">
         <v>2029</v>
       </c>
@@ -9150,7 +9460,7 @@
         <v>37.808466184234931</v>
       </c>
     </row>
-    <row r="54" spans="4:5" x14ac:dyDescent="0.75">
+    <row r="54" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D54" s="30">
         <v>2030</v>
       </c>
@@ -9159,7 +9469,7 @@
         <v>40.099753413934195</v>
       </c>
     </row>
-    <row r="55" spans="4:5" x14ac:dyDescent="0.75">
+    <row r="55" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D55" s="33">
         <v>2031</v>
       </c>
@@ -9168,7 +9478,7 @@
         <v>40.099753413934195</v>
       </c>
     </row>
-    <row r="56" spans="4:5" x14ac:dyDescent="0.75">
+    <row r="56" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D56" s="33">
         <v>2032</v>
       </c>
@@ -9177,7 +9487,7 @@
         <v>40.099753413934195</v>
       </c>
     </row>
-    <row r="57" spans="4:5" x14ac:dyDescent="0.75">
+    <row r="57" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D57" s="33">
         <v>2033</v>
       </c>
@@ -9186,7 +9496,7 @@
         <v>40.099753413934195</v>
       </c>
     </row>
-    <row r="58" spans="4:5" x14ac:dyDescent="0.75">
+    <row r="58" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D58" s="33">
         <v>2034</v>
       </c>
@@ -9195,7 +9505,7 @@
         <v>40.099753413934195</v>
       </c>
     </row>
-    <row r="59" spans="4:5" x14ac:dyDescent="0.75">
+    <row r="59" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D59" s="33">
         <v>2035</v>
       </c>
@@ -9204,7 +9514,7 @@
         <v>40.099753413934195</v>
       </c>
     </row>
-    <row r="60" spans="4:5" x14ac:dyDescent="0.75">
+    <row r="60" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D60" s="33">
         <v>2036</v>
       </c>
@@ -9213,7 +9523,7 @@
         <v>40.099753413934195</v>
       </c>
     </row>
-    <row r="61" spans="4:5" x14ac:dyDescent="0.75">
+    <row r="61" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D61" s="33">
         <v>2037</v>
       </c>
@@ -9222,7 +9532,7 @@
         <v>40.099753413934195</v>
       </c>
     </row>
-    <row r="62" spans="4:5" x14ac:dyDescent="0.75">
+    <row r="62" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D62" s="33">
         <v>2038</v>
       </c>
@@ -9231,7 +9541,7 @@
         <v>40.099753413934195</v>
       </c>
     </row>
-    <row r="63" spans="4:5" x14ac:dyDescent="0.75">
+    <row r="63" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D63" s="33">
         <v>2039</v>
       </c>
@@ -9240,7 +9550,7 @@
         <v>40.099753413934195</v>
       </c>
     </row>
-    <row r="64" spans="4:5" x14ac:dyDescent="0.75">
+    <row r="64" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D64" s="33">
         <v>2040</v>
       </c>
@@ -9249,7 +9559,7 @@
         <v>40.099753413934195</v>
       </c>
     </row>
-    <row r="65" spans="4:5" x14ac:dyDescent="0.75">
+    <row r="65" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D65" s="33">
         <v>2041</v>
       </c>
@@ -9258,7 +9568,7 @@
         <v>40.099753413934195</v>
       </c>
     </row>
-    <row r="66" spans="4:5" x14ac:dyDescent="0.75">
+    <row r="66" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D66" s="33">
         <v>2042</v>
       </c>
@@ -9267,7 +9577,7 @@
         <v>40.099753413934195</v>
       </c>
     </row>
-    <row r="67" spans="4:5" x14ac:dyDescent="0.75">
+    <row r="67" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D67" s="33">
         <v>2043</v>
       </c>
@@ -9276,7 +9586,7 @@
         <v>40.099753413934195</v>
       </c>
     </row>
-    <row r="68" spans="4:5" x14ac:dyDescent="0.75">
+    <row r="68" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D68" s="33">
         <v>2044</v>
       </c>
@@ -9285,7 +9595,7 @@
         <v>40.099753413934195</v>
       </c>
     </row>
-    <row r="69" spans="4:5" x14ac:dyDescent="0.75">
+    <row r="69" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D69" s="33">
         <v>2045</v>
       </c>
@@ -9294,7 +9604,7 @@
         <v>40.099753413934195</v>
       </c>
     </row>
-    <row r="70" spans="4:5" x14ac:dyDescent="0.75">
+    <row r="70" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D70" s="33">
         <v>2046</v>
       </c>
@@ -9303,7 +9613,7 @@
         <v>40.099753413934195</v>
       </c>
     </row>
-    <row r="71" spans="4:5" x14ac:dyDescent="0.75">
+    <row r="71" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D71" s="33">
         <v>2047</v>
       </c>
@@ -9312,7 +9622,7 @@
         <v>40.099753413934195</v>
       </c>
     </row>
-    <row r="72" spans="4:5" x14ac:dyDescent="0.75">
+    <row r="72" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D72" s="33">
         <v>2048</v>
       </c>
@@ -9321,7 +9631,7 @@
         <v>40.099753413934195</v>
       </c>
     </row>
-    <row r="73" spans="4:5" x14ac:dyDescent="0.75">
+    <row r="73" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D73" s="33">
         <v>2049</v>
       </c>
@@ -9330,7 +9640,7 @@
         <v>40.099753413934195</v>
       </c>
     </row>
-    <row r="74" spans="4:5" x14ac:dyDescent="0.75">
+    <row r="74" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D74" s="33">
         <v>2050</v>
       </c>
@@ -9344,20 +9654,20 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E803D18-8E69-4DA2-A8FF-24AA4A9E4E5D}">
-  <dimension ref="A2:AG22"/>
+  <dimension ref="A2:AH29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.2">
       <c r="C2">
         <v>2020</v>
       </c>
@@ -9452,7 +9762,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A3" s="32" t="s">
         <v>5</v>
       </c>
@@ -9554,7 +9864,7 @@
         <v>44.815360675261218</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A4" s="32" t="s">
         <v>5</v>
       </c>
@@ -9686,7 +9996,7 @@
         <v>44.815360675261218</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A5" s="32" t="s">
         <v>5</v>
       </c>
@@ -9818,7 +10128,7 @@
         <v>44.815360675261218</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A6" s="32" t="s">
         <v>5</v>
       </c>
@@ -9950,7 +10260,7 @@
         <v>44.815360675261218</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A7" s="32" t="s">
         <v>5</v>
       </c>
@@ -10082,7 +10392,7 @@
         <v>44.815360675261218</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A8" s="32" t="s">
         <v>5</v>
       </c>
@@ -10214,7 +10524,7 @@
         <v>44.815360675261218</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A9" s="32" t="s">
         <v>5</v>
       </c>
@@ -10346,7 +10656,7 @@
         <v>44.815360675261218</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A10" s="32" t="s">
         <v>5</v>
       </c>
@@ -10478,7 +10788,7 @@
         <v>44.815360675261218</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A11" s="32" t="s">
         <v>5</v>
       </c>
@@ -10610,7 +10920,7 @@
         <v>44.815360675261218</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A12" s="32" t="s">
         <v>5</v>
       </c>
@@ -10742,7 +11052,7 @@
         <v>44.815360675261218</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A13" s="32" t="s">
         <v>5</v>
       </c>
@@ -10874,7 +11184,7 @@
         <v>44.815360675261218</v>
       </c>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A14" s="32" t="s">
         <v>5</v>
       </c>
@@ -11006,7 +11316,7 @@
         <v>44.815360675261218</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A15" s="34" t="s">
         <v>4</v>
       </c>
@@ -11108,7 +11418,7 @@
         <v>40.099753413934195</v>
       </c>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A16" s="34" t="s">
         <v>5</v>
       </c>
@@ -11240,7 +11550,7 @@
         <v>40.099753413934195</v>
       </c>
     </row>
-    <row r="17" spans="1:33" x14ac:dyDescent="0.75">
+    <row r="17" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A17" s="34" t="s">
         <v>6</v>
       </c>
@@ -11372,7 +11682,7 @@
         <v>40.099753413934195</v>
       </c>
     </row>
-    <row r="18" spans="1:33" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A18" s="34" t="s">
         <v>7</v>
       </c>
@@ -11504,7 +11814,7 @@
         <v>40.099753413934195</v>
       </c>
     </row>
-    <row r="19" spans="1:33" x14ac:dyDescent="0.75">
+    <row r="19" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A19" s="34" t="s">
         <v>8</v>
       </c>
@@ -11636,7 +11946,7 @@
         <v>40.099753413934195</v>
       </c>
     </row>
-    <row r="20" spans="1:33" x14ac:dyDescent="0.75">
+    <row r="20" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A20" s="34" t="s">
         <v>9</v>
       </c>
@@ -11768,7 +12078,7 @@
         <v>40.099753413934195</v>
       </c>
     </row>
-    <row r="21" spans="1:33" x14ac:dyDescent="0.75">
+    <row r="21" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A21" s="34" t="s">
         <v>10</v>
       </c>
@@ -11900,7 +12210,7 @@
         <v>40.099753413934195</v>
       </c>
     </row>
-    <row r="22" spans="1:33" x14ac:dyDescent="0.75">
+    <row r="22" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A22" s="34" t="s">
         <v>11</v>
       </c>
@@ -12030,6 +12340,912 @@
       <c r="AG22">
         <f t="shared" si="32"/>
         <v>40.099753413934195</v>
+      </c>
+    </row>
+    <row r="23" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A23" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" s="38" t="s">
+        <v>157</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <f>WA!B2</f>
+        <v>58</v>
+      </c>
+      <c r="G23">
+        <f>WA!C2</f>
+        <v>64</v>
+      </c>
+      <c r="H23">
+        <f>WA!D2</f>
+        <v>70</v>
+      </c>
+      <c r="I23">
+        <f>WA!E2</f>
+        <v>76</v>
+      </c>
+      <c r="J23">
+        <f>WA!F2</f>
+        <v>82</v>
+      </c>
+      <c r="K23">
+        <f>WA!G2</f>
+        <v>88</v>
+      </c>
+      <c r="L23">
+        <f>WA!H2</f>
+        <v>94</v>
+      </c>
+      <c r="M23">
+        <f>WA!I2</f>
+        <v>100</v>
+      </c>
+      <c r="N23">
+        <f>WA!J2</f>
+        <v>100</v>
+      </c>
+      <c r="O23">
+        <f>WA!K2</f>
+        <v>100</v>
+      </c>
+      <c r="P23">
+        <f>WA!L2</f>
+        <v>100</v>
+      </c>
+      <c r="Q23">
+        <f>WA!M2</f>
+        <v>100</v>
+      </c>
+      <c r="R23">
+        <f>WA!N2</f>
+        <v>58</v>
+      </c>
+      <c r="S23">
+        <f>WA!O2</f>
+        <v>54.4</v>
+      </c>
+      <c r="T23">
+        <f>WA!P2</f>
+        <v>50.8</v>
+      </c>
+      <c r="U23">
+        <f>WA!Q2</f>
+        <v>47.2</v>
+      </c>
+      <c r="V23">
+        <f>WA!R2</f>
+        <v>43.6</v>
+      </c>
+      <c r="W23">
+        <f>WA!S2</f>
+        <v>40</v>
+      </c>
+      <c r="X23">
+        <f>WA!T2</f>
+        <v>44</v>
+      </c>
+      <c r="Y23">
+        <f>WA!U2</f>
+        <v>48</v>
+      </c>
+      <c r="Z23">
+        <f>WA!V2</f>
+        <v>52</v>
+      </c>
+      <c r="AA23">
+        <f>WA!W2</f>
+        <v>56</v>
+      </c>
+      <c r="AB23">
+        <f>WA!X2</f>
+        <v>60</v>
+      </c>
+      <c r="AC23">
+        <f>WA!Y2</f>
+        <v>64</v>
+      </c>
+      <c r="AD23">
+        <f>WA!Z2</f>
+        <v>68</v>
+      </c>
+      <c r="AE23">
+        <f>WA!AA2</f>
+        <v>72</v>
+      </c>
+      <c r="AF23">
+        <f>WA!AB2</f>
+        <v>76</v>
+      </c>
+      <c r="AG23">
+        <f>WA!AC2</f>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="24" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A24" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" s="38" t="s">
+        <v>157</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <f>F23</f>
+        <v>58</v>
+      </c>
+      <c r="G24">
+        <f t="shared" ref="G24:AG24" si="34">G23</f>
+        <v>64</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="34"/>
+        <v>70</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="34"/>
+        <v>76</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="34"/>
+        <v>82</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="34"/>
+        <v>88</v>
+      </c>
+      <c r="L24">
+        <f t="shared" si="34"/>
+        <v>94</v>
+      </c>
+      <c r="M24">
+        <f t="shared" si="34"/>
+        <v>100</v>
+      </c>
+      <c r="N24">
+        <f t="shared" si="34"/>
+        <v>100</v>
+      </c>
+      <c r="O24">
+        <f t="shared" si="34"/>
+        <v>100</v>
+      </c>
+      <c r="P24">
+        <f t="shared" si="34"/>
+        <v>100</v>
+      </c>
+      <c r="Q24">
+        <f t="shared" si="34"/>
+        <v>100</v>
+      </c>
+      <c r="R24">
+        <f t="shared" si="34"/>
+        <v>58</v>
+      </c>
+      <c r="S24">
+        <f t="shared" si="34"/>
+        <v>54.4</v>
+      </c>
+      <c r="T24">
+        <f t="shared" si="34"/>
+        <v>50.8</v>
+      </c>
+      <c r="U24">
+        <f t="shared" si="34"/>
+        <v>47.2</v>
+      </c>
+      <c r="V24">
+        <f t="shared" si="34"/>
+        <v>43.6</v>
+      </c>
+      <c r="W24">
+        <f t="shared" si="34"/>
+        <v>40</v>
+      </c>
+      <c r="X24">
+        <f t="shared" si="34"/>
+        <v>44</v>
+      </c>
+      <c r="Y24">
+        <f t="shared" si="34"/>
+        <v>48</v>
+      </c>
+      <c r="Z24">
+        <f t="shared" si="34"/>
+        <v>52</v>
+      </c>
+      <c r="AA24">
+        <f t="shared" si="34"/>
+        <v>56</v>
+      </c>
+      <c r="AB24">
+        <f t="shared" si="34"/>
+        <v>60</v>
+      </c>
+      <c r="AC24">
+        <f t="shared" si="34"/>
+        <v>64</v>
+      </c>
+      <c r="AD24">
+        <f t="shared" si="34"/>
+        <v>68</v>
+      </c>
+      <c r="AE24">
+        <f t="shared" si="34"/>
+        <v>72</v>
+      </c>
+      <c r="AF24">
+        <f t="shared" si="34"/>
+        <v>76</v>
+      </c>
+      <c r="AG24">
+        <f t="shared" si="34"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="25" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A25" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" s="38" t="s">
+        <v>157</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <f>F23</f>
+        <v>58</v>
+      </c>
+      <c r="G25">
+        <f t="shared" ref="G25:AG25" si="35">G23</f>
+        <v>64</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="35"/>
+        <v>70</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="35"/>
+        <v>76</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="35"/>
+        <v>82</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="35"/>
+        <v>88</v>
+      </c>
+      <c r="L25">
+        <f t="shared" si="35"/>
+        <v>94</v>
+      </c>
+      <c r="M25">
+        <f t="shared" si="35"/>
+        <v>100</v>
+      </c>
+      <c r="N25">
+        <f t="shared" si="35"/>
+        <v>100</v>
+      </c>
+      <c r="O25">
+        <f t="shared" si="35"/>
+        <v>100</v>
+      </c>
+      <c r="P25">
+        <f t="shared" si="35"/>
+        <v>100</v>
+      </c>
+      <c r="Q25">
+        <f t="shared" si="35"/>
+        <v>100</v>
+      </c>
+      <c r="R25">
+        <f t="shared" si="35"/>
+        <v>58</v>
+      </c>
+      <c r="S25">
+        <f t="shared" si="35"/>
+        <v>54.4</v>
+      </c>
+      <c r="T25">
+        <f t="shared" si="35"/>
+        <v>50.8</v>
+      </c>
+      <c r="U25">
+        <f t="shared" si="35"/>
+        <v>47.2</v>
+      </c>
+      <c r="V25">
+        <f t="shared" si="35"/>
+        <v>43.6</v>
+      </c>
+      <c r="W25">
+        <f t="shared" si="35"/>
+        <v>40</v>
+      </c>
+      <c r="X25">
+        <f t="shared" si="35"/>
+        <v>44</v>
+      </c>
+      <c r="Y25">
+        <f t="shared" si="35"/>
+        <v>48</v>
+      </c>
+      <c r="Z25">
+        <f t="shared" si="35"/>
+        <v>52</v>
+      </c>
+      <c r="AA25">
+        <f t="shared" si="35"/>
+        <v>56</v>
+      </c>
+      <c r="AB25">
+        <f t="shared" si="35"/>
+        <v>60</v>
+      </c>
+      <c r="AC25">
+        <f t="shared" si="35"/>
+        <v>64</v>
+      </c>
+      <c r="AD25">
+        <f t="shared" si="35"/>
+        <v>68</v>
+      </c>
+      <c r="AE25">
+        <f t="shared" si="35"/>
+        <v>72</v>
+      </c>
+      <c r="AF25">
+        <f t="shared" si="35"/>
+        <v>76</v>
+      </c>
+      <c r="AG25">
+        <f t="shared" si="35"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="26" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A26" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26" s="38" t="s">
+        <v>157</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <f>WA!B4</f>
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <f>WA!C4</f>
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <f>WA!D4</f>
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <f>WA!E4</f>
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <f>WA!F4</f>
+        <v>0</v>
+      </c>
+      <c r="K26">
+        <f>WA!G4</f>
+        <v>0</v>
+      </c>
+      <c r="L26">
+        <f>WA!H4</f>
+        <v>0</v>
+      </c>
+      <c r="M26">
+        <f>WA!I4</f>
+        <v>0</v>
+      </c>
+      <c r="N26">
+        <f>WA!J4</f>
+        <v>0</v>
+      </c>
+      <c r="O26">
+        <f>WA!K4</f>
+        <v>0</v>
+      </c>
+      <c r="P26">
+        <f>WA!L4</f>
+        <v>0</v>
+      </c>
+      <c r="Q26">
+        <f t="shared" ref="Q26:AF26" si="36">Q24</f>
+        <v>100</v>
+      </c>
+      <c r="R26">
+        <f t="shared" si="36"/>
+        <v>58</v>
+      </c>
+      <c r="S26">
+        <f t="shared" si="36"/>
+        <v>54.4</v>
+      </c>
+      <c r="T26">
+        <f t="shared" si="36"/>
+        <v>50.8</v>
+      </c>
+      <c r="U26">
+        <f t="shared" si="36"/>
+        <v>47.2</v>
+      </c>
+      <c r="V26">
+        <f t="shared" si="36"/>
+        <v>43.6</v>
+      </c>
+      <c r="W26">
+        <f t="shared" si="36"/>
+        <v>40</v>
+      </c>
+      <c r="X26">
+        <f t="shared" si="36"/>
+        <v>44</v>
+      </c>
+      <c r="Y26">
+        <f t="shared" si="36"/>
+        <v>48</v>
+      </c>
+      <c r="Z26">
+        <f t="shared" si="36"/>
+        <v>52</v>
+      </c>
+      <c r="AA26">
+        <f t="shared" si="36"/>
+        <v>56</v>
+      </c>
+      <c r="AB26">
+        <f t="shared" si="36"/>
+        <v>60</v>
+      </c>
+      <c r="AC26">
+        <f t="shared" si="36"/>
+        <v>64</v>
+      </c>
+      <c r="AD26">
+        <f t="shared" si="36"/>
+        <v>68</v>
+      </c>
+      <c r="AE26">
+        <f t="shared" si="36"/>
+        <v>72</v>
+      </c>
+      <c r="AF26">
+        <f t="shared" si="36"/>
+        <v>76</v>
+      </c>
+      <c r="AG26">
+        <f t="shared" ref="AG26" si="37">AG24</f>
+        <v>80</v>
+      </c>
+      <c r="AH26" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="27" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A27" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" s="38" t="s">
+        <v>157</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <f>F23</f>
+        <v>58</v>
+      </c>
+      <c r="G27">
+        <f t="shared" ref="G27:AG27" si="38">G23</f>
+        <v>64</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="38"/>
+        <v>70</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="38"/>
+        <v>76</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="38"/>
+        <v>82</v>
+      </c>
+      <c r="K27">
+        <f t="shared" si="38"/>
+        <v>88</v>
+      </c>
+      <c r="L27">
+        <f t="shared" si="38"/>
+        <v>94</v>
+      </c>
+      <c r="M27">
+        <f t="shared" si="38"/>
+        <v>100</v>
+      </c>
+      <c r="N27">
+        <f t="shared" si="38"/>
+        <v>100</v>
+      </c>
+      <c r="O27">
+        <f t="shared" si="38"/>
+        <v>100</v>
+      </c>
+      <c r="P27">
+        <f t="shared" si="38"/>
+        <v>100</v>
+      </c>
+      <c r="Q27">
+        <f t="shared" si="38"/>
+        <v>100</v>
+      </c>
+      <c r="R27">
+        <f t="shared" si="38"/>
+        <v>58</v>
+      </c>
+      <c r="S27">
+        <f t="shared" si="38"/>
+        <v>54.4</v>
+      </c>
+      <c r="T27">
+        <f t="shared" si="38"/>
+        <v>50.8</v>
+      </c>
+      <c r="U27">
+        <f t="shared" si="38"/>
+        <v>47.2</v>
+      </c>
+      <c r="V27">
+        <f t="shared" si="38"/>
+        <v>43.6</v>
+      </c>
+      <c r="W27">
+        <f t="shared" si="38"/>
+        <v>40</v>
+      </c>
+      <c r="X27">
+        <f t="shared" si="38"/>
+        <v>44</v>
+      </c>
+      <c r="Y27">
+        <f t="shared" si="38"/>
+        <v>48</v>
+      </c>
+      <c r="Z27">
+        <f t="shared" si="38"/>
+        <v>52</v>
+      </c>
+      <c r="AA27">
+        <f t="shared" si="38"/>
+        <v>56</v>
+      </c>
+      <c r="AB27">
+        <f t="shared" si="38"/>
+        <v>60</v>
+      </c>
+      <c r="AC27">
+        <f t="shared" si="38"/>
+        <v>64</v>
+      </c>
+      <c r="AD27">
+        <f t="shared" si="38"/>
+        <v>68</v>
+      </c>
+      <c r="AE27">
+        <f t="shared" si="38"/>
+        <v>72</v>
+      </c>
+      <c r="AF27">
+        <f t="shared" si="38"/>
+        <v>76</v>
+      </c>
+      <c r="AG27">
+        <f t="shared" si="38"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="28" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A28" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="B28" s="38" t="s">
+        <v>157</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <f>F23</f>
+        <v>58</v>
+      </c>
+      <c r="G28">
+        <f t="shared" ref="G28:AG29" si="39">G23</f>
+        <v>64</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="39"/>
+        <v>70</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="39"/>
+        <v>76</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="39"/>
+        <v>82</v>
+      </c>
+      <c r="K28">
+        <f t="shared" si="39"/>
+        <v>88</v>
+      </c>
+      <c r="L28">
+        <f t="shared" si="39"/>
+        <v>94</v>
+      </c>
+      <c r="M28">
+        <f t="shared" si="39"/>
+        <v>100</v>
+      </c>
+      <c r="N28">
+        <f t="shared" si="39"/>
+        <v>100</v>
+      </c>
+      <c r="O28">
+        <f t="shared" si="39"/>
+        <v>100</v>
+      </c>
+      <c r="P28">
+        <f t="shared" si="39"/>
+        <v>100</v>
+      </c>
+      <c r="Q28">
+        <f t="shared" si="39"/>
+        <v>100</v>
+      </c>
+      <c r="R28">
+        <f t="shared" si="39"/>
+        <v>58</v>
+      </c>
+      <c r="S28">
+        <f t="shared" si="39"/>
+        <v>54.4</v>
+      </c>
+      <c r="T28">
+        <f t="shared" si="39"/>
+        <v>50.8</v>
+      </c>
+      <c r="U28">
+        <f t="shared" si="39"/>
+        <v>47.2</v>
+      </c>
+      <c r="V28">
+        <f t="shared" si="39"/>
+        <v>43.6</v>
+      </c>
+      <c r="W28">
+        <f t="shared" si="39"/>
+        <v>40</v>
+      </c>
+      <c r="X28">
+        <f t="shared" si="39"/>
+        <v>44</v>
+      </c>
+      <c r="Y28">
+        <f t="shared" si="39"/>
+        <v>48</v>
+      </c>
+      <c r="Z28">
+        <f t="shared" si="39"/>
+        <v>52</v>
+      </c>
+      <c r="AA28">
+        <f t="shared" si="39"/>
+        <v>56</v>
+      </c>
+      <c r="AB28">
+        <f t="shared" si="39"/>
+        <v>60</v>
+      </c>
+      <c r="AC28">
+        <f t="shared" si="39"/>
+        <v>64</v>
+      </c>
+      <c r="AD28">
+        <f t="shared" si="39"/>
+        <v>68</v>
+      </c>
+      <c r="AE28">
+        <f t="shared" si="39"/>
+        <v>72</v>
+      </c>
+      <c r="AF28">
+        <f t="shared" si="39"/>
+        <v>76</v>
+      </c>
+      <c r="AG28">
+        <f t="shared" si="39"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="29" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A29" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="B29" s="38" t="s">
+        <v>157</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <f>F24</f>
+        <v>58</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="39"/>
+        <v>64</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="39"/>
+        <v>70</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="39"/>
+        <v>76</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="39"/>
+        <v>82</v>
+      </c>
+      <c r="K29">
+        <f t="shared" si="39"/>
+        <v>88</v>
+      </c>
+      <c r="L29">
+        <f t="shared" si="39"/>
+        <v>94</v>
+      </c>
+      <c r="M29">
+        <f t="shared" si="39"/>
+        <v>100</v>
+      </c>
+      <c r="N29">
+        <f t="shared" si="39"/>
+        <v>100</v>
+      </c>
+      <c r="O29">
+        <f t="shared" si="39"/>
+        <v>100</v>
+      </c>
+      <c r="P29">
+        <f t="shared" si="39"/>
+        <v>100</v>
+      </c>
+      <c r="Q29">
+        <f t="shared" si="39"/>
+        <v>100</v>
+      </c>
+      <c r="R29">
+        <f t="shared" si="39"/>
+        <v>58</v>
+      </c>
+      <c r="S29">
+        <f t="shared" si="39"/>
+        <v>54.4</v>
+      </c>
+      <c r="T29">
+        <f t="shared" si="39"/>
+        <v>50.8</v>
+      </c>
+      <c r="U29">
+        <f t="shared" si="39"/>
+        <v>47.2</v>
+      </c>
+      <c r="V29">
+        <f t="shared" si="39"/>
+        <v>43.6</v>
+      </c>
+      <c r="W29">
+        <f t="shared" si="39"/>
+        <v>40</v>
+      </c>
+      <c r="X29">
+        <f t="shared" si="39"/>
+        <v>44</v>
+      </c>
+      <c r="Y29">
+        <f t="shared" si="39"/>
+        <v>48</v>
+      </c>
+      <c r="Z29">
+        <f t="shared" si="39"/>
+        <v>52</v>
+      </c>
+      <c r="AA29">
+        <f t="shared" si="39"/>
+        <v>56</v>
+      </c>
+      <c r="AB29">
+        <f t="shared" si="39"/>
+        <v>60</v>
+      </c>
+      <c r="AC29">
+        <f t="shared" si="39"/>
+        <v>64</v>
+      </c>
+      <c r="AD29">
+        <f t="shared" si="39"/>
+        <v>68</v>
+      </c>
+      <c r="AE29">
+        <f t="shared" si="39"/>
+        <v>72</v>
+      </c>
+      <c r="AF29">
+        <f t="shared" si="39"/>
+        <v>76</v>
+      </c>
+      <c r="AG29">
+        <f t="shared" si="39"/>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -12038,23 +13254,23 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A588720-4507-45D9-BCC3-2B2208374E22}">
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:AF9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="48" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -12152,7 +13368,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -12177,111 +13393,85 @@
         <v>0</v>
       </c>
       <c r="G2" s="35">
-        <f>SUMIFS('state calcs'!H:H,'state calcs'!$A:$A,$A2,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="H2" s="35">
-        <f>SUMIFS('state calcs'!I:I,'state calcs'!$A:$A,$A2,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="I2" s="35">
-        <f>SUMIFS('state calcs'!J:J,'state calcs'!$A:$A,$A2,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="J2" s="35">
-        <f>SUMIFS('state calcs'!K:K,'state calcs'!$A:$A,$A2,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="K2" s="35">
-        <f>SUMIFS('state calcs'!L:L,'state calcs'!$A:$A,$A2,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="L2" s="35">
-        <f>SUMIFS('state calcs'!M:M,'state calcs'!$A:$A,$A2,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="M2" s="35">
-        <f>SUMIFS('state calcs'!N:N,'state calcs'!$A:$A,$A2,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="N2" s="35">
-        <f>SUMIFS('state calcs'!O:O,'state calcs'!$A:$A,$A2,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="O2" s="35">
-        <f>SUMIFS('state calcs'!P:P,'state calcs'!$A:$A,$A2,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="P2" s="35">
-        <f>SUMIFS('state calcs'!Q:Q,'state calcs'!$A:$A,$A2,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="Q2" s="35">
-        <f>SUMIFS('state calcs'!R:R,'state calcs'!$A:$A,$A2,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="R2" s="35">
-        <f>SUMIFS('state calcs'!S:S,'state calcs'!$A:$A,$A2,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="S2" s="35">
-        <f>SUMIFS('state calcs'!T:T,'state calcs'!$A:$A,$A2,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="T2" s="35">
-        <f>SUMIFS('state calcs'!U:U,'state calcs'!$A:$A,$A2,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="U2" s="35">
-        <f>SUMIFS('state calcs'!V:V,'state calcs'!$A:$A,$A2,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="V2" s="35">
-        <f>SUMIFS('state calcs'!W:W,'state calcs'!$A:$A,$A2,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="W2" s="35">
-        <f>SUMIFS('state calcs'!X:X,'state calcs'!$A:$A,$A2,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="X2" s="35">
-        <f>SUMIFS('state calcs'!Y:Y,'state calcs'!$A:$A,$A2,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="Y2" s="35">
-        <f>SUMIFS('state calcs'!Z:Z,'state calcs'!$A:$A,$A2,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="Z2" s="35">
-        <f>SUMIFS('state calcs'!AA:AA,'state calcs'!$A:$A,$A2,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="AA2" s="35">
-        <f>SUMIFS('state calcs'!AB:AB,'state calcs'!$A:$A,$A2,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="AB2" s="35">
-        <f>SUMIFS('state calcs'!AC:AC,'state calcs'!$A:$A,$A2,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="AC2" s="35">
-        <f>SUMIFS('state calcs'!AD:AD,'state calcs'!$A:$A,$A2,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="AD2" s="35">
-        <f>SUMIFS('state calcs'!AE:AE,'state calcs'!$A:$A,$A2,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="AE2" s="35">
-        <f>SUMIFS('state calcs'!AF:AF,'state calcs'!$A:$A,$A2,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="AF2" s="35">
-        <f>SUMIFS('state calcs'!AG:AG,'state calcs'!$A:$A,$A2,'state calcs'!$B:$B,About!$B$2)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -12306,111 +13496,85 @@
         <v>11.092397772593358</v>
       </c>
       <c r="G3" s="35">
-        <f>SUMIFS('state calcs'!H:H,'state calcs'!$A:$A,$A3,'state calcs'!$B:$B,About!$B$2)</f>
-        <v>12.389434807311318</v>
+        <v>0</v>
       </c>
       <c r="H3" s="35">
-        <f>SUMIFS('state calcs'!I:I,'state calcs'!$A:$A,$A3,'state calcs'!$B:$B,About!$B$2)</f>
-        <v>13.686471842029277</v>
+        <v>0</v>
       </c>
       <c r="I3" s="35">
-        <f>SUMIFS('state calcs'!J:J,'state calcs'!$A:$A,$A3,'state calcs'!$B:$B,About!$B$2)</f>
-        <v>14.983508876747237</v>
+        <v>0</v>
       </c>
       <c r="J3" s="35">
-        <f>SUMIFS('state calcs'!K:K,'state calcs'!$A:$A,$A3,'state calcs'!$B:$B,About!$B$2)</f>
-        <v>16.280545911465197</v>
+        <v>0</v>
       </c>
       <c r="K3" s="35">
-        <f>SUMIFS('state calcs'!L:L,'state calcs'!$A:$A,$A3,'state calcs'!$B:$B,About!$B$2)</f>
-        <v>17.577582946183611</v>
+        <v>0</v>
       </c>
       <c r="L3" s="35">
-        <f>SUMIFS('state calcs'!M:M,'state calcs'!$A:$A,$A3,'state calcs'!$B:$B,About!$B$2)</f>
-        <v>18.874619980901571</v>
+        <v>0</v>
       </c>
       <c r="M3" s="35">
-        <f>SUMIFS('state calcs'!N:N,'state calcs'!$A:$A,$A3,'state calcs'!$B:$B,About!$B$2)</f>
-        <v>20.17165701561953</v>
+        <v>0</v>
       </c>
       <c r="N3" s="35">
-        <f>SUMIFS('state calcs'!O:O,'state calcs'!$A:$A,$A3,'state calcs'!$B:$B,About!$B$2)</f>
-        <v>21.46869405033749</v>
+        <v>0</v>
       </c>
       <c r="O3" s="35">
-        <f>SUMIFS('state calcs'!P:P,'state calcs'!$A:$A,$A3,'state calcs'!$B:$B,About!$B$2)</f>
-        <v>22.76573108505545</v>
+        <v>0</v>
       </c>
       <c r="P3" s="35">
-        <f>SUMIFS('state calcs'!Q:Q,'state calcs'!$A:$A,$A3,'state calcs'!$B:$B,About!$B$2)</f>
-        <v>24.062768119773409</v>
+        <v>0</v>
       </c>
       <c r="Q3" s="35">
-        <f>SUMIFS('state calcs'!R:R,'state calcs'!$A:$A,$A3,'state calcs'!$B:$B,About!$B$2)</f>
-        <v>25.359805154491369</v>
+        <v>0</v>
       </c>
       <c r="R3" s="35">
-        <f>SUMIFS('state calcs'!S:S,'state calcs'!$A:$A,$A3,'state calcs'!$B:$B,About!$B$2)</f>
-        <v>26.656842189209328</v>
+        <v>0</v>
       </c>
       <c r="S3" s="35">
-        <f>SUMIFS('state calcs'!T:T,'state calcs'!$A:$A,$A3,'state calcs'!$B:$B,About!$B$2)</f>
-        <v>27.953879223927288</v>
+        <v>0</v>
       </c>
       <c r="T3" s="35">
-        <f>SUMIFS('state calcs'!U:U,'state calcs'!$A:$A,$A3,'state calcs'!$B:$B,About!$B$2)</f>
-        <v>29.250916258645248</v>
+        <v>0</v>
       </c>
       <c r="U3" s="35">
-        <f>SUMIFS('state calcs'!V:V,'state calcs'!$A:$A,$A3,'state calcs'!$B:$B,About!$B$2)</f>
-        <v>30.547953293363207</v>
+        <v>0</v>
       </c>
       <c r="V3" s="35">
-        <f>SUMIFS('state calcs'!W:W,'state calcs'!$A:$A,$A3,'state calcs'!$B:$B,About!$B$2)</f>
-        <v>31.844990328081167</v>
+        <v>0</v>
       </c>
       <c r="W3" s="35">
-        <f>SUMIFS('state calcs'!X:X,'state calcs'!$A:$A,$A3,'state calcs'!$B:$B,About!$B$2)</f>
-        <v>33.142027362799126</v>
+        <v>0</v>
       </c>
       <c r="X3" s="35">
-        <f>SUMIFS('state calcs'!Y:Y,'state calcs'!$A:$A,$A3,'state calcs'!$B:$B,About!$B$2)</f>
-        <v>34.439064397517541</v>
+        <v>0</v>
       </c>
       <c r="Y3" s="35">
-        <f>SUMIFS('state calcs'!Z:Z,'state calcs'!$A:$A,$A3,'state calcs'!$B:$B,About!$B$2)</f>
-        <v>35.7361014322355</v>
+        <v>0</v>
       </c>
       <c r="Z3" s="35">
-        <f>SUMIFS('state calcs'!AA:AA,'state calcs'!$A:$A,$A3,'state calcs'!$B:$B,About!$B$2)</f>
-        <v>37.03313846695346</v>
+        <v>0</v>
       </c>
       <c r="AA3" s="35">
-        <f>SUMIFS('state calcs'!AB:AB,'state calcs'!$A:$A,$A3,'state calcs'!$B:$B,About!$B$2)</f>
-        <v>38.33017550167142</v>
+        <v>0</v>
       </c>
       <c r="AB3" s="35">
-        <f>SUMIFS('state calcs'!AC:AC,'state calcs'!$A:$A,$A3,'state calcs'!$B:$B,About!$B$2)</f>
-        <v>39.627212536389379</v>
+        <v>0</v>
       </c>
       <c r="AC3" s="35">
-        <f>SUMIFS('state calcs'!AD:AD,'state calcs'!$A:$A,$A3,'state calcs'!$B:$B,About!$B$2)</f>
-        <v>40.924249571107339</v>
+        <v>0</v>
       </c>
       <c r="AD3" s="35">
-        <f>SUMIFS('state calcs'!AE:AE,'state calcs'!$A:$A,$A3,'state calcs'!$B:$B,About!$B$2)</f>
-        <v>42.221286605825298</v>
+        <v>0</v>
       </c>
       <c r="AE3" s="35">
-        <f>SUMIFS('state calcs'!AF:AF,'state calcs'!$A:$A,$A3,'state calcs'!$B:$B,About!$B$2)</f>
-        <v>43.518323640543258</v>
+        <v>0</v>
       </c>
       <c r="AF3" s="35">
-        <f>SUMIFS('state calcs'!AG:AG,'state calcs'!$A:$A,$A3,'state calcs'!$B:$B,About!$B$2)</f>
-        <v>44.815360675261218</v>
-      </c>
-    </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -12435,111 +13599,85 @@
         <v>0</v>
       </c>
       <c r="G4" s="35">
-        <f>SUMIFS('state calcs'!H:H,'state calcs'!$A:$A,$A4,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="H4" s="35">
-        <f>SUMIFS('state calcs'!I:I,'state calcs'!$A:$A,$A4,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="I4" s="35">
-        <f>SUMIFS('state calcs'!J:J,'state calcs'!$A:$A,$A4,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="J4" s="35">
-        <f>SUMIFS('state calcs'!K:K,'state calcs'!$A:$A,$A4,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="K4" s="35">
-        <f>SUMIFS('state calcs'!L:L,'state calcs'!$A:$A,$A4,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="L4" s="35">
-        <f>SUMIFS('state calcs'!M:M,'state calcs'!$A:$A,$A4,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="M4" s="35">
-        <f>SUMIFS('state calcs'!N:N,'state calcs'!$A:$A,$A4,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="N4" s="35">
-        <f>SUMIFS('state calcs'!O:O,'state calcs'!$A:$A,$A4,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="O4" s="35">
-        <f>SUMIFS('state calcs'!P:P,'state calcs'!$A:$A,$A4,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="P4" s="35">
-        <f>SUMIFS('state calcs'!Q:Q,'state calcs'!$A:$A,$A4,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="Q4" s="35">
-        <f>SUMIFS('state calcs'!R:R,'state calcs'!$A:$A,$A4,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="R4" s="35">
-        <f>SUMIFS('state calcs'!S:S,'state calcs'!$A:$A,$A4,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="S4" s="35">
-        <f>SUMIFS('state calcs'!T:T,'state calcs'!$A:$A,$A4,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="T4" s="35">
-        <f>SUMIFS('state calcs'!U:U,'state calcs'!$A:$A,$A4,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="U4" s="35">
-        <f>SUMIFS('state calcs'!V:V,'state calcs'!$A:$A,$A4,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="V4" s="35">
-        <f>SUMIFS('state calcs'!W:W,'state calcs'!$A:$A,$A4,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="W4" s="35">
-        <f>SUMIFS('state calcs'!X:X,'state calcs'!$A:$A,$A4,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="X4" s="35">
-        <f>SUMIFS('state calcs'!Y:Y,'state calcs'!$A:$A,$A4,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="Y4" s="35">
-        <f>SUMIFS('state calcs'!Z:Z,'state calcs'!$A:$A,$A4,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="Z4" s="35">
-        <f>SUMIFS('state calcs'!AA:AA,'state calcs'!$A:$A,$A4,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="AA4" s="35">
-        <f>SUMIFS('state calcs'!AB:AB,'state calcs'!$A:$A,$A4,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="AB4" s="35">
-        <f>SUMIFS('state calcs'!AC:AC,'state calcs'!$A:$A,$A4,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="AC4" s="35">
-        <f>SUMIFS('state calcs'!AD:AD,'state calcs'!$A:$A,$A4,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="AD4" s="35">
-        <f>SUMIFS('state calcs'!AE:AE,'state calcs'!$A:$A,$A4,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="AE4" s="35">
-        <f>SUMIFS('state calcs'!AF:AF,'state calcs'!$A:$A,$A4,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="AF4" s="35">
-        <f>SUMIFS('state calcs'!AG:AG,'state calcs'!$A:$A,$A4,'state calcs'!$B:$B,About!$B$2)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -12564,111 +13702,85 @@
         <v>0</v>
       </c>
       <c r="G5" s="35">
-        <f>SUMIFS('state calcs'!H:H,'state calcs'!$A:$A,$A5,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="H5" s="35">
-        <f>SUMIFS('state calcs'!I:I,'state calcs'!$A:$A,$A5,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="I5" s="35">
-        <f>SUMIFS('state calcs'!J:J,'state calcs'!$A:$A,$A5,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="J5" s="35">
-        <f>SUMIFS('state calcs'!K:K,'state calcs'!$A:$A,$A5,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="K5" s="35">
-        <f>SUMIFS('state calcs'!L:L,'state calcs'!$A:$A,$A5,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="L5" s="35">
-        <f>SUMIFS('state calcs'!M:M,'state calcs'!$A:$A,$A5,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="M5" s="35">
-        <f>SUMIFS('state calcs'!N:N,'state calcs'!$A:$A,$A5,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="N5" s="35">
-        <f>SUMIFS('state calcs'!O:O,'state calcs'!$A:$A,$A5,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="O5" s="35">
-        <f>SUMIFS('state calcs'!P:P,'state calcs'!$A:$A,$A5,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="P5" s="35">
-        <f>SUMIFS('state calcs'!Q:Q,'state calcs'!$A:$A,$A5,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="Q5" s="35">
-        <f>SUMIFS('state calcs'!R:R,'state calcs'!$A:$A,$A5,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="R5" s="35">
-        <f>SUMIFS('state calcs'!S:S,'state calcs'!$A:$A,$A5,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="S5" s="35">
-        <f>SUMIFS('state calcs'!T:T,'state calcs'!$A:$A,$A5,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="T5" s="35">
-        <f>SUMIFS('state calcs'!U:U,'state calcs'!$A:$A,$A5,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="U5" s="35">
-        <f>SUMIFS('state calcs'!V:V,'state calcs'!$A:$A,$A5,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="V5" s="35">
-        <f>SUMIFS('state calcs'!W:W,'state calcs'!$A:$A,$A5,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="W5" s="35">
-        <f>SUMIFS('state calcs'!X:X,'state calcs'!$A:$A,$A5,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="X5" s="35">
-        <f>SUMIFS('state calcs'!Y:Y,'state calcs'!$A:$A,$A5,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="Y5" s="35">
-        <f>SUMIFS('state calcs'!Z:Z,'state calcs'!$A:$A,$A5,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="Z5" s="35">
-        <f>SUMIFS('state calcs'!AA:AA,'state calcs'!$A:$A,$A5,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="AA5" s="35">
-        <f>SUMIFS('state calcs'!AB:AB,'state calcs'!$A:$A,$A5,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="AB5" s="35">
-        <f>SUMIFS('state calcs'!AC:AC,'state calcs'!$A:$A,$A5,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="AC5" s="35">
-        <f>SUMIFS('state calcs'!AD:AD,'state calcs'!$A:$A,$A5,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="AD5" s="35">
-        <f>SUMIFS('state calcs'!AE:AE,'state calcs'!$A:$A,$A5,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="AE5" s="35">
-        <f>SUMIFS('state calcs'!AF:AF,'state calcs'!$A:$A,$A5,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="AF5" s="35">
-        <f>SUMIFS('state calcs'!AG:AG,'state calcs'!$A:$A,$A5,'state calcs'!$B:$B,About!$B$2)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -12693,111 +13805,85 @@
         <v>0</v>
       </c>
       <c r="G6" s="35">
-        <f>SUMIFS('state calcs'!H:H,'state calcs'!$A:$A,$A6,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="H6" s="35">
-        <f>SUMIFS('state calcs'!I:I,'state calcs'!$A:$A,$A6,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="I6" s="35">
-        <f>SUMIFS('state calcs'!J:J,'state calcs'!$A:$A,$A6,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="J6" s="35">
-        <f>SUMIFS('state calcs'!K:K,'state calcs'!$A:$A,$A6,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="K6" s="35">
-        <f>SUMIFS('state calcs'!L:L,'state calcs'!$A:$A,$A6,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="L6" s="35">
-        <f>SUMIFS('state calcs'!M:M,'state calcs'!$A:$A,$A6,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="M6" s="35">
-        <f>SUMIFS('state calcs'!N:N,'state calcs'!$A:$A,$A6,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="N6" s="35">
-        <f>SUMIFS('state calcs'!O:O,'state calcs'!$A:$A,$A6,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="O6" s="35">
-        <f>SUMIFS('state calcs'!P:P,'state calcs'!$A:$A,$A6,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="P6" s="35">
-        <f>SUMIFS('state calcs'!Q:Q,'state calcs'!$A:$A,$A6,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="Q6" s="35">
-        <f>SUMIFS('state calcs'!R:R,'state calcs'!$A:$A,$A6,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="R6" s="35">
-        <f>SUMIFS('state calcs'!S:S,'state calcs'!$A:$A,$A6,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="S6" s="35">
-        <f>SUMIFS('state calcs'!T:T,'state calcs'!$A:$A,$A6,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="T6" s="35">
-        <f>SUMIFS('state calcs'!U:U,'state calcs'!$A:$A,$A6,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="U6" s="35">
-        <f>SUMIFS('state calcs'!V:V,'state calcs'!$A:$A,$A6,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="V6" s="35">
-        <f>SUMIFS('state calcs'!W:W,'state calcs'!$A:$A,$A6,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="W6" s="35">
-        <f>SUMIFS('state calcs'!X:X,'state calcs'!$A:$A,$A6,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="X6" s="35">
-        <f>SUMIFS('state calcs'!Y:Y,'state calcs'!$A:$A,$A6,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="Y6" s="35">
-        <f>SUMIFS('state calcs'!Z:Z,'state calcs'!$A:$A,$A6,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="Z6" s="35">
-        <f>SUMIFS('state calcs'!AA:AA,'state calcs'!$A:$A,$A6,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="AA6" s="35">
-        <f>SUMIFS('state calcs'!AB:AB,'state calcs'!$A:$A,$A6,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="AB6" s="35">
-        <f>SUMIFS('state calcs'!AC:AC,'state calcs'!$A:$A,$A6,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="AC6" s="35">
-        <f>SUMIFS('state calcs'!AD:AD,'state calcs'!$A:$A,$A6,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="AD6" s="35">
-        <f>SUMIFS('state calcs'!AE:AE,'state calcs'!$A:$A,$A6,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="AE6" s="35">
-        <f>SUMIFS('state calcs'!AF:AF,'state calcs'!$A:$A,$A6,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="AF6" s="35">
-        <f>SUMIFS('state calcs'!AG:AG,'state calcs'!$A:$A,$A6,'state calcs'!$B:$B,About!$B$2)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -12822,111 +13908,85 @@
         <v>0</v>
       </c>
       <c r="G7" s="35">
-        <f>SUMIFS('state calcs'!H:H,'state calcs'!$A:$A,$A7,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="H7" s="35">
-        <f>SUMIFS('state calcs'!I:I,'state calcs'!$A:$A,$A7,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="I7" s="35">
-        <f>SUMIFS('state calcs'!J:J,'state calcs'!$A:$A,$A7,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="J7" s="35">
-        <f>SUMIFS('state calcs'!K:K,'state calcs'!$A:$A,$A7,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="K7" s="35">
-        <f>SUMIFS('state calcs'!L:L,'state calcs'!$A:$A,$A7,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="L7" s="35">
-        <f>SUMIFS('state calcs'!M:M,'state calcs'!$A:$A,$A7,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="M7" s="35">
-        <f>SUMIFS('state calcs'!N:N,'state calcs'!$A:$A,$A7,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="N7" s="35">
-        <f>SUMIFS('state calcs'!O:O,'state calcs'!$A:$A,$A7,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="O7" s="35">
-        <f>SUMIFS('state calcs'!P:P,'state calcs'!$A:$A,$A7,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="P7" s="35">
-        <f>SUMIFS('state calcs'!Q:Q,'state calcs'!$A:$A,$A7,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="Q7" s="35">
-        <f>SUMIFS('state calcs'!R:R,'state calcs'!$A:$A,$A7,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="R7" s="35">
-        <f>SUMIFS('state calcs'!S:S,'state calcs'!$A:$A,$A7,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="S7" s="35">
-        <f>SUMIFS('state calcs'!T:T,'state calcs'!$A:$A,$A7,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="T7" s="35">
-        <f>SUMIFS('state calcs'!U:U,'state calcs'!$A:$A,$A7,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="U7" s="35">
-        <f>SUMIFS('state calcs'!V:V,'state calcs'!$A:$A,$A7,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="V7" s="35">
-        <f>SUMIFS('state calcs'!W:W,'state calcs'!$A:$A,$A7,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="W7" s="35">
-        <f>SUMIFS('state calcs'!X:X,'state calcs'!$A:$A,$A7,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="X7" s="35">
-        <f>SUMIFS('state calcs'!Y:Y,'state calcs'!$A:$A,$A7,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="Y7" s="35">
-        <f>SUMIFS('state calcs'!Z:Z,'state calcs'!$A:$A,$A7,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="Z7" s="35">
-        <f>SUMIFS('state calcs'!AA:AA,'state calcs'!$A:$A,$A7,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="AA7" s="35">
-        <f>SUMIFS('state calcs'!AB:AB,'state calcs'!$A:$A,$A7,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="AB7" s="35">
-        <f>SUMIFS('state calcs'!AC:AC,'state calcs'!$A:$A,$A7,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="AC7" s="35">
-        <f>SUMIFS('state calcs'!AD:AD,'state calcs'!$A:$A,$A7,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="AD7" s="35">
-        <f>SUMIFS('state calcs'!AE:AE,'state calcs'!$A:$A,$A7,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="AE7" s="35">
-        <f>SUMIFS('state calcs'!AF:AF,'state calcs'!$A:$A,$A7,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="AF7" s="35">
-        <f>SUMIFS('state calcs'!AG:AG,'state calcs'!$A:$A,$A7,'state calcs'!$B:$B,About!$B$2)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -12951,111 +14011,85 @@
         <v>0</v>
       </c>
       <c r="G8" s="35">
-        <f>SUMIFS('state calcs'!H:H,'state calcs'!$A:$A,$A8,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="H8" s="35">
-        <f>SUMIFS('state calcs'!I:I,'state calcs'!$A:$A,$A8,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="I8" s="35">
-        <f>SUMIFS('state calcs'!J:J,'state calcs'!$A:$A,$A8,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="J8" s="35">
-        <f>SUMIFS('state calcs'!K:K,'state calcs'!$A:$A,$A8,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="K8" s="35">
-        <f>SUMIFS('state calcs'!L:L,'state calcs'!$A:$A,$A8,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="L8" s="35">
-        <f>SUMIFS('state calcs'!M:M,'state calcs'!$A:$A,$A8,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="M8" s="35">
-        <f>SUMIFS('state calcs'!N:N,'state calcs'!$A:$A,$A8,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="N8" s="35">
-        <f>SUMIFS('state calcs'!O:O,'state calcs'!$A:$A,$A8,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="O8" s="35">
-        <f>SUMIFS('state calcs'!P:P,'state calcs'!$A:$A,$A8,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="P8" s="35">
-        <f>SUMIFS('state calcs'!Q:Q,'state calcs'!$A:$A,$A8,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="Q8" s="35">
-        <f>SUMIFS('state calcs'!R:R,'state calcs'!$A:$A,$A8,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="R8" s="35">
-        <f>SUMIFS('state calcs'!S:S,'state calcs'!$A:$A,$A8,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="S8" s="35">
-        <f>SUMIFS('state calcs'!T:T,'state calcs'!$A:$A,$A8,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="T8" s="35">
-        <f>SUMIFS('state calcs'!U:U,'state calcs'!$A:$A,$A8,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="U8" s="35">
-        <f>SUMIFS('state calcs'!V:V,'state calcs'!$A:$A,$A8,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="V8" s="35">
-        <f>SUMIFS('state calcs'!W:W,'state calcs'!$A:$A,$A8,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="W8" s="35">
-        <f>SUMIFS('state calcs'!X:X,'state calcs'!$A:$A,$A8,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="X8" s="35">
-        <f>SUMIFS('state calcs'!Y:Y,'state calcs'!$A:$A,$A8,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="Y8" s="35">
-        <f>SUMIFS('state calcs'!Z:Z,'state calcs'!$A:$A,$A8,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="Z8" s="35">
-        <f>SUMIFS('state calcs'!AA:AA,'state calcs'!$A:$A,$A8,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="AA8" s="35">
-        <f>SUMIFS('state calcs'!AB:AB,'state calcs'!$A:$A,$A8,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="AB8" s="35">
-        <f>SUMIFS('state calcs'!AC:AC,'state calcs'!$A:$A,$A8,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="AC8" s="35">
-        <f>SUMIFS('state calcs'!AD:AD,'state calcs'!$A:$A,$A8,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="AD8" s="35">
-        <f>SUMIFS('state calcs'!AE:AE,'state calcs'!$A:$A,$A8,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="AE8" s="35">
-        <f>SUMIFS('state calcs'!AF:AF,'state calcs'!$A:$A,$A8,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="AF8" s="35">
-        <f>SUMIFS('state calcs'!AG:AG,'state calcs'!$A:$A,$A8,'state calcs'!$B:$B,About!$B$2)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -13080,107 +14114,81 @@
         <v>0</v>
       </c>
       <c r="G9" s="35">
-        <f>SUMIFS('state calcs'!H:H,'state calcs'!$A:$A,$A9,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="H9" s="35">
-        <f>SUMIFS('state calcs'!I:I,'state calcs'!$A:$A,$A9,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="I9" s="35">
-        <f>SUMIFS('state calcs'!J:J,'state calcs'!$A:$A,$A9,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="J9" s="35">
-        <f>SUMIFS('state calcs'!K:K,'state calcs'!$A:$A,$A9,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="K9" s="35">
-        <f>SUMIFS('state calcs'!L:L,'state calcs'!$A:$A,$A9,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="L9" s="35">
-        <f>SUMIFS('state calcs'!M:M,'state calcs'!$A:$A,$A9,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="M9" s="35">
-        <f>SUMIFS('state calcs'!N:N,'state calcs'!$A:$A,$A9,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="N9" s="35">
-        <f>SUMIFS('state calcs'!O:O,'state calcs'!$A:$A,$A9,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="O9" s="35">
-        <f>SUMIFS('state calcs'!P:P,'state calcs'!$A:$A,$A9,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="P9" s="35">
-        <f>SUMIFS('state calcs'!Q:Q,'state calcs'!$A:$A,$A9,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="Q9" s="35">
-        <f>SUMIFS('state calcs'!R:R,'state calcs'!$A:$A,$A9,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="R9" s="35">
-        <f>SUMIFS('state calcs'!S:S,'state calcs'!$A:$A,$A9,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="S9" s="35">
-        <f>SUMIFS('state calcs'!T:T,'state calcs'!$A:$A,$A9,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="T9" s="35">
-        <f>SUMIFS('state calcs'!U:U,'state calcs'!$A:$A,$A9,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="U9" s="35">
-        <f>SUMIFS('state calcs'!V:V,'state calcs'!$A:$A,$A9,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="V9" s="35">
-        <f>SUMIFS('state calcs'!W:W,'state calcs'!$A:$A,$A9,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="W9" s="35">
-        <f>SUMIFS('state calcs'!X:X,'state calcs'!$A:$A,$A9,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="X9" s="35">
-        <f>SUMIFS('state calcs'!Y:Y,'state calcs'!$A:$A,$A9,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="Y9" s="35">
-        <f>SUMIFS('state calcs'!Z:Z,'state calcs'!$A:$A,$A9,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="Z9" s="35">
-        <f>SUMIFS('state calcs'!AA:AA,'state calcs'!$A:$A,$A9,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="AA9" s="35">
-        <f>SUMIFS('state calcs'!AB:AB,'state calcs'!$A:$A,$A9,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="AB9" s="35">
-        <f>SUMIFS('state calcs'!AC:AC,'state calcs'!$A:$A,$A9,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="AC9" s="35">
-        <f>SUMIFS('state calcs'!AD:AD,'state calcs'!$A:$A,$A9,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="AD9" s="35">
-        <f>SUMIFS('state calcs'!AE:AE,'state calcs'!$A:$A,$A9,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="AE9" s="35">
-        <f>SUMIFS('state calcs'!AF:AF,'state calcs'!$A:$A,$A9,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
       <c r="AF9" s="35">
-        <f>SUMIFS('state calcs'!AG:AG,'state calcs'!$A:$A,$A9,'state calcs'!$B:$B,About!$B$2)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>